<commit_message>
Minor changes to the way years are handled in the .xlsx
</commit_message>
<xml_diff>
--- a/src/template/Regnskap_template.xlsx
+++ b/src/template/Regnskap_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Kristent\Misjonskirka\Div\python_script\src\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Kristent\Misjonskirka\Regnskap\python_script\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D747B8-6390-4E6C-9158-A73910D27318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FFBBA4-610A-499B-BE5D-5F1FAC564990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regnskap" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Dato</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>Signatur:</t>
-  </si>
-  <si>
-    <t>Kasserer for Filter</t>
   </si>
   <si>
     <t>____________________________________________</t>
@@ -912,7 +909,9 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -935,7 +934,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
@@ -962,10 +961,10 @@
         <v>3</v>
       </c>
       <c r="I2" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="40" t="s">
         <v>25</v>
-      </c>
-      <c r="J2" s="40" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
@@ -994,7 +993,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="3"/>
@@ -1016,7 +1015,7 @@
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6"/>
       <c r="H5" s="2"/>
@@ -1052,7 +1051,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1060,13 +1059,14 @@
         <v>22</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
-      <c r="B9" s="34" t="s">
-        <v>23</v>
+      <c r="B9" s="34" t="str">
+        <f>CONCATENATE("Kasserer for ", MID(Regnskap!B1, 10, 1000))</f>
+        <v xml:space="preserve">Kasserer for FILTER </v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBF28CE-3AC6-4D68-A5F3-A708FFB83CF7}">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1119,8 +1121,8 @@
         <v>Inngående balanse 01.01.ÅRSTALL</v>
       </c>
       <c r="C3" s="22" t="str">
-        <f>Regnskap!D4</f>
-        <v>FYLL INN</v>
+        <f>IF(Regnskap!D4="FYLL INN","Se hovedark",Regnskap!D4)</f>
+        <v>Se hovedark</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="12"/>
@@ -1416,8 +1418,8 @@
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="18" t="str">
-        <f>Regnskap!E5</f>
-        <v>FYLL INN</v>
+        <f>IF(Regnskap!E5="FYLL INN","Se hovedark",Regnskap!E5)</f>
+        <v>Se hovedark</v>
       </c>
       <c r="E29" s="12"/>
     </row>
@@ -1485,10 +1487,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1496,10 +1498,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,10 +1509,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1518,10 +1520,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1529,10 +1531,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1540,10 +1542,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,10 +1553,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,10 +1564,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1573,10 +1575,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1584,7 +1586,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1592,7 +1594,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v1.6: Don't add transactions older than the oldest one already in the spreadsheet. Minor improvement to the xlsx template. If Ref. And num.ref. are both present, don't compare the date.
</commit_message>
<xml_diff>
--- a/src/template/Regnskap_template.xlsx
+++ b/src/template/Regnskap_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\Documents\_My_files\Kristent\Misjonskirka\Regnskap\python_script\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FFBBA4-610A-499B-BE5D-5F1FAC564990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC8CB0C-7DCC-4C19-ACCC-C2CA6553D865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="731" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regnskap" sheetId="1" r:id="rId1"/>
@@ -409,9 +409,6 @@
     <xf numFmtId="5" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -480,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,7 +578,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Hvis du legger til nye kategorier i regnerarket "Kategorier", sett in tomme rader i tabellen til venstre, i oversikten</a:t>
+            <a:t>Hvis du legger til nye kategorier i regnerarket "Kategorier", sett in tomme rader i tabellen til venstre, nederst i oversikten</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nb-NO" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -910,7 +910,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -930,72 +930,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="39" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="str">
+      <c r="A4" s="23" t="str">
         <f>CONCATENATE("01.01.", C1)</f>
         <v>01.01.ÅRSTALL</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1003,18 +1003,18 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="str">
+      <c r="A5" s="23" t="str">
         <f>CONCATENATE("31.12.", C1)</f>
         <v>31.12.ÅRSTALL</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="39" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="38" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="6"/>
@@ -1023,18 +1023,18 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <f>SUM(D$4:D5)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <f>SUM(E$4:E5)</f>
         <v>0</v>
       </c>
@@ -1047,24 +1047,24 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34" t="str">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33" t="str">
         <f>CONCATENATE("Kasserer for ", MID(Regnskap!B1, 10, 1000))</f>
         <v xml:space="preserve">Kasserer for FILTER </v>
       </c>
@@ -1084,9 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBF28CE-3AC6-4D68-A5F3-A708FFB83CF7}">
   <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1096,21 +1094,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="22.2" x14ac:dyDescent="0.35">
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="44" t="str">
         <f>CONCATENATE("Årsregnskap ", Regnskap!C1, " for ", MID(Regnskap!B1, 10, 1000))</f>
         <v xml:space="preserve">Årsregnskap ÅRSTALL for FILTER </v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="12"/>
@@ -1120,9 +1118,9 @@
         <f>CONCATENATE("Inngående balanse ", Regnskap!A4)</f>
         <v>Inngående balanse 01.01.ÅRSTALL</v>
       </c>
-      <c r="C3" s="22" t="str">
-        <f>IF(Regnskap!D4="FYLL INN","Se hovedark",Regnskap!D4)</f>
-        <v>Se hovedark</v>
+      <c r="C3" s="45" t="str">
+        <f>IF(Regnskap!D4="FYLL INN","Fyll inn i hovedark",Regnskap!D4)</f>
+        <v>Fyll inn i hovedark</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="12"/>
@@ -1418,8 +1416,8 @@
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="18" t="str">
-        <f>IF(Regnskap!E5="FYLL INN","Se hovedark",Regnskap!E5)</f>
-        <v>Se hovedark</v>
+        <f>IF(Regnskap!E5="FYLL INN","Fyll inn i hovedark",Regnskap!E5)</f>
+        <v>Fyll inn i hovedark</v>
       </c>
       <c r="E29" s="12"/>
     </row>
@@ -1467,7 +1465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60601A7-F667-4E03-ADA6-BD5B7CDBF2BF}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>